<commit_message>
Fixed issues with comma floating point numbers, added feature name generation, added formating for txt file output
</commit_message>
<xml_diff>
--- a/DigitalSignalProcessing/FeaturesInformativeness/app/app/core/resources/Th.xlsx
+++ b/DigitalSignalProcessing/FeaturesInformativeness/app/app/core/resources/Th.xlsx
@@ -506,9 +506,6 @@
     <t>Ew details 7 lvl</t>
   </si>
   <si>
-    <t>Ew details 8 lvl.</t>
-  </si>
-  <si>
     <t>Ew approx 1 lvl</t>
   </si>
   <si>
@@ -521,25 +518,28 @@
     <t>Ew approx 4 lvl</t>
   </si>
   <si>
+    <t>Ew approx 6 lvl</t>
+  </si>
+  <si>
+    <t>Ew approx 7 lvl</t>
+  </si>
+  <si>
+    <t>Ew approx 8 lvl</t>
+  </si>
+  <si>
+    <t>AutoCorrelation offset 1</t>
+  </si>
+  <si>
+    <t>AutoCorrelation offset 3</t>
+  </si>
+  <si>
+    <t>AutoCorrelation offset 2</t>
+  </si>
+  <si>
     <t>Ew approx 5 lvl</t>
   </si>
   <si>
-    <t>Ew approx 6 lvl</t>
-  </si>
-  <si>
-    <t>Ew approx 7 lvl</t>
-  </si>
-  <si>
-    <t>Ew approx 8 lvl</t>
-  </si>
-  <si>
-    <t>AutoCorrelation offset 1</t>
-  </si>
-  <si>
-    <t>AutoCorrelation offset 2</t>
-  </si>
-  <si>
-    <t>AutoCorrelation offset 3</t>
+    <t>Ew details 8 lvl</t>
   </si>
 </sst>
 </file>
@@ -869,7 +869,7 @@
   <dimension ref="A1:V9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -914,40 +914,40 @@
         <v>159</v>
       </c>
       <c r="K1" t="s">
+        <v>171</v>
+      </c>
+      <c r="L1" t="s">
         <v>160</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>161</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>162</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>163</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>170</v>
+      </c>
+      <c r="Q1" t="s">
         <v>164</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>165</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>166</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="V1" s="1" t="s">
         <v>168</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>170</v>
-      </c>
-      <c r="V1" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="2" spans="1:22" x14ac:dyDescent="0.25">

</xml_diff>